<commit_message>
Update MIMXRT1064 MCU Module - FOOTPRINTS CHECK.xlsx
</commit_message>
<xml_diff>
--- a/CHECK SHEETS/MIMXRT1064 MCU Module - FOOTPRINTS CHECK.xlsx
+++ b/CHECK SHEETS/MIMXRT1064 MCU Module - FOOTPRINTS CHECK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32470\Documents\GitHub\MIMXRT1064-MCU-Module\CHECK SHEETS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1630E6E-67A1-43FB-A1D1-0C878EB58AC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFEA5A5-80F1-4FE4-A29E-33E1EB29AD0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,7 +229,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,12 +332,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FF34A853"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -366,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -404,7 +398,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -629,10 +622,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:XFD45"/>
+  <dimension ref="A1:XFD51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -649,14 +642,14 @@
   <sheetData>
     <row r="1" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="11"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" s="12" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -682,15 +675,15 @@
       </c>
     </row>
     <row r="3" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
@@ -803,15 +796,15 @@
       <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
@@ -924,15 +917,15 @@
       <c r="G24" s="15"/>
     </row>
     <row r="25" spans="1:16384" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
     </row>
     <row r="26" spans="1:16384" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -50110,15 +50103,15 @@
       </c>
     </row>
     <row r="30" spans="1:16384" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
     </row>
     <row r="31" spans="1:16384" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
@@ -50132,15 +50125,15 @@
       <c r="G31" s="15"/>
     </row>
     <row r="32" spans="1:16384" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
     </row>
     <row r="33" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
@@ -50198,26 +50191,26 @@
       <c r="G37" s="26"/>
     </row>
     <row r="38" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
     </row>
     <row r="39" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
     </row>
     <row r="40" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
@@ -50253,18 +50246,18 @@
       <c r="G42" s="26"/>
     </row>
     <row r="43" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
     </row>
     <row r="44" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="29" t="s">
         <v>38</v>
       </c>
       <c r="B44" s="26"/>
@@ -50285,6 +50278,12 @@
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
     </row>
+    <row r="46" spans="1:7" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:7" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:7" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A32:G32"/>

</xml_diff>